<commit_message>
rewrote file importers to be more generalized and user-friendly, all reference ids can be found through the ui and excel column data is more obvious. round trip upload, download working for all files
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/initialDataFiles/prescriptions.xlsx
+++ b/backend/src/main/resources/initialDataFiles/prescriptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\medtracker_v2_rest_api\backend\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2E9552-EC9A-487D-9622-6C2CDA01E82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F0746F-062C-4CCE-A3EA-E0EF4E3160CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{D62EB2BE-1EF4-4692-9FA4-4C3CA6687488}"/>
+    <workbookView xWindow="65220" yWindow="8580" windowWidth="23676" windowHeight="16200" xr2:uid="{D62EB2BE-1EF4-4692-9FA4-4C3CA6687488}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t xml:space="preserve"> MEDICATION_ID</t>
   </si>
@@ -46,6 +43,15 @@
   </si>
   <si>
     <t xml:space="preserve"> DOSE_MG</t>
+  </si>
+  <si>
+    <t>Day Stages</t>
+  </si>
+  <si>
+    <t>MORNING,MIDDAY</t>
+  </si>
+  <si>
+    <t>doc1@medtracker.com</t>
   </si>
 </sst>
 </file>
@@ -55,7 +61,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm:ss\.ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,16 +70,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFBCBEC4"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF6AAB73"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,21 +95,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -423,21 +423,21 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" customWidth="1"/>
+    <col min="4" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -459,90 +459,102 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" s="3">
+      <c r="B2" s="1">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45583</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45589.999305555553</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="4">
-        <v>45583</v>
-      </c>
-      <c r="F2" s="4">
-        <v>45589.999305555553</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45590</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45597.5</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>45590</v>
-      </c>
-      <c r="F3" s="4">
-        <v>45597.5</v>
-      </c>
-      <c r="G3">
-        <v>200</v>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45597.541666666664</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45613.999305555553</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>45597.541666666664</v>
-      </c>
-      <c r="F4" s="4">
-        <v>45613.999305555553</v>
-      </c>
-      <c r="G4">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
         <v>45621</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5">
-        <v>175</v>
+      <c r="E5" s="2"/>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{38485F6C-6067-4659-8EFA-C5B3A37AEBBB}"/>
+    <hyperlink ref="C3:C5" r:id="rId2" display="doc1@medtracker.com" xr:uid="{720AD874-025C-4B16-9796-45C307E1D547}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>